<commit_message>
Atualização das Tabelas e correção do Gap
</commit_message>
<xml_diff>
--- a/Tabelas.xlsx
+++ b/Tabelas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="569">
   <si>
     <t>Jorge ILS</t>
   </si>
@@ -1671,12 +1671,6 @@
     <t>Tabela 2</t>
   </si>
   <si>
-    <t>Gap (BEP)</t>
-  </si>
-  <si>
-    <t>Gap (EEP)</t>
-  </si>
-  <si>
     <t>R-BEP (min)</t>
   </si>
   <si>
@@ -1689,12 +1683,6 @@
     <t>R-EEP (média)</t>
   </si>
   <si>
-    <t>Tabela 3</t>
-  </si>
-  <si>
-    <t>Tabela 4</t>
-  </si>
-  <si>
     <t>R-EEP (nédia)</t>
   </si>
   <si>
@@ -1705,6 +1693,39 @@
   </si>
   <si>
     <t>Tabela 6</t>
+  </si>
+  <si>
+    <t>Gap(R-BEP)</t>
+  </si>
+  <si>
+    <t>Gap(R-EEP)</t>
+  </si>
+  <si>
+    <t>R-BEP</t>
+  </si>
+  <si>
+    <t>R-EEP</t>
+  </si>
+  <si>
+    <t>BEP x Moreno</t>
+  </si>
+  <si>
+    <t>EEP x Moreno</t>
+  </si>
+  <si>
+    <t>ganhou</t>
+  </si>
+  <si>
+    <t>perdeu</t>
+  </si>
+  <si>
+    <t>empatou</t>
+  </si>
+  <si>
+    <t>RBEP x Moreno</t>
+  </si>
+  <si>
+    <t>REEP x Moreno</t>
   </si>
 </sst>
 </file>
@@ -1751,7 +1772,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1759,6 +1780,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -76071,7 +76094,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P201"/>
   <sheetViews>
-    <sheetView topLeftCell="A160" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="N185" activeCellId="1" sqref="J185 N185"/>
     </sheetView>
   </sheetViews>
@@ -83920,30 +83943,39 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T18"/>
+  <dimension ref="A1:W22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:Q18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:23">
       <c r="A1" t="s">
         <v>544</v>
       </c>
-      <c r="J1" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20">
+    </row>
+    <row r="2" spans="1:23">
       <c r="A2" s="5" t="s">
         <v>545</v>
       </c>
@@ -83963,39 +83995,38 @@
         <v>4</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>550</v>
+        <v>560</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>551</v>
-      </c>
-      <c r="I2" s="5"/>
+        <v>561</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>558</v>
+      </c>
       <c r="J2" s="5" t="s">
-        <v>545</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>546</v>
-      </c>
+        <v>559</v>
+      </c>
+      <c r="K2" s="5"/>
       <c r="L2" s="5" t="s">
-        <v>2</v>
+        <v>562</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>4</v>
+        <v>563</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>554</v>
+        <v>567</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>555</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>552</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>553</v>
-      </c>
+        <v>568</v>
+      </c>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
       <c r="S2" s="5"/>
-    </row>
-    <row r="3" spans="1:20">
+      <c r="T2" s="5"/>
+      <c r="V2" s="5"/>
+    </row>
+    <row r="3" spans="1:23">
       <c r="A3">
         <v>20</v>
       </c>
@@ -84005,53 +84036,56 @@
       <c r="C3" s="1">
         <v>0.8</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="8">
         <v>1.04</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="8">
         <v>1.08</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="8">
         <v>1.04</v>
       </c>
-      <c r="G3" s="4">
-        <f>(E3-C3)/C3*100</f>
-        <v>35</v>
-      </c>
-      <c r="H3" s="4">
-        <f>(F3-C3)/C3*100</f>
-        <v>30</v>
-      </c>
-      <c r="I3" s="5"/>
-      <c r="J3">
-        <v>20</v>
-      </c>
-      <c r="K3" s="1">
-        <v>41.8</v>
-      </c>
-      <c r="L3" s="1">
-        <v>1.08</v>
-      </c>
-      <c r="M3" s="4">
-        <v>1.04</v>
-      </c>
-      <c r="N3" s="4">
-        <v>1.4979999999999998</v>
+      <c r="G3" s="7">
+        <v>0.84</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0.84</v>
+      </c>
+      <c r="I3" s="4">
+        <f>(G3-C3)/C3*100</f>
+        <v>4.9999999999999902</v>
+      </c>
+      <c r="J3" s="4">
+        <f>(H3-C3)/C3*100</f>
+        <v>4.9999999999999902</v>
+      </c>
+      <c r="K3" s="5"/>
+      <c r="L3" s="2">
+        <f>E3-D3</f>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="M3" s="1">
+        <f>F3-D3</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="1">
+        <f>G3-D3</f>
+        <v>-0.20000000000000007</v>
       </c>
       <c r="O3" s="4">
-        <v>1.5783999999999991</v>
-      </c>
-      <c r="P3" s="3">
-        <v>0.84</v>
-      </c>
-      <c r="Q3" s="3">
-        <v>0.84</v>
-      </c>
-      <c r="R3" s="1"/>
+        <f>H3-D3</f>
+        <v>-0.20000000000000007</v>
+      </c>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
       <c r="S3" s="3"/>
-      <c r="T3" s="2"/>
-    </row>
-    <row r="4" spans="1:20">
+      <c r="T3" s="3"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="2"/>
+    </row>
+    <row r="4" spans="1:23">
       <c r="A4">
         <v>40</v>
       </c>
@@ -84061,53 +84095,56 @@
       <c r="C4" s="1">
         <v>2.8</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="8">
         <v>3.76</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="8">
         <v>3.84</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="8">
         <v>3.68</v>
       </c>
-      <c r="G4" s="4">
-        <f t="shared" ref="G4:G18" si="0">(E4-C4)/C4*100</f>
-        <v>37.142857142857146</v>
-      </c>
-      <c r="H4" s="4">
-        <f t="shared" ref="H4:H18" si="1">(F4-C4)/C4*100</f>
-        <v>31.428571428571445</v>
-      </c>
-      <c r="I4" s="5"/>
-      <c r="J4">
-        <v>40</v>
-      </c>
-      <c r="K4" s="1">
-        <v>70.8</v>
-      </c>
-      <c r="L4" s="1">
-        <v>3.84</v>
-      </c>
-      <c r="M4" s="4">
-        <v>3.68</v>
-      </c>
-      <c r="N4" s="4">
-        <v>4.7128000000000014</v>
+      <c r="G4" s="7">
+        <v>3.28</v>
+      </c>
+      <c r="H4" s="8">
+        <v>3.48</v>
+      </c>
+      <c r="I4" s="4">
+        <f t="shared" ref="I4:I18" si="0">(G4-C4)/C4*100</f>
+        <v>17.142857142857142</v>
+      </c>
+      <c r="J4" s="4">
+        <f t="shared" ref="J4:J18" si="1">(H4-C4)/C4*100</f>
+        <v>24.285714285714295</v>
+      </c>
+      <c r="K4" s="5"/>
+      <c r="L4" s="2">
+        <f t="shared" ref="L4:L18" si="2">E4-D4</f>
+        <v>8.0000000000000071E-2</v>
+      </c>
+      <c r="M4" s="1">
+        <f t="shared" ref="M4:M18" si="3">F4-D4</f>
+        <v>-7.9999999999999627E-2</v>
+      </c>
+      <c r="N4" s="1">
+        <f t="shared" ref="N4:N18" si="4">G4-D4</f>
+        <v>-0.48</v>
       </c>
       <c r="O4" s="4">
-        <v>4.8152000000000008</v>
-      </c>
-      <c r="P4" s="3">
-        <v>3.28</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>3.48</v>
-      </c>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="2"/>
-    </row>
-    <row r="5" spans="1:20">
+        <f t="shared" ref="O4:O18" si="5">H4-D4</f>
+        <v>-0.2799999999999998</v>
+      </c>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="2"/>
+    </row>
+    <row r="5" spans="1:23">
       <c r="A5">
         <v>60</v>
       </c>
@@ -84117,53 +84154,56 @@
       <c r="C5" s="1">
         <v>6.3</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="8">
         <v>8.16</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="8">
         <v>7.72</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="8">
         <v>7.8</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="7">
+        <v>7.12</v>
+      </c>
+      <c r="H5" s="8">
+        <v>7.32</v>
+      </c>
+      <c r="I5" s="4">
         <f t="shared" si="0"/>
-        <v>22.539682539682541</v>
-      </c>
-      <c r="H5" s="4">
+        <v>13.015873015873019</v>
+      </c>
+      <c r="J5" s="4">
         <f t="shared" si="1"/>
-        <v>23.80952380952381</v>
-      </c>
-      <c r="I5" s="5"/>
-      <c r="J5">
-        <v>60</v>
-      </c>
-      <c r="K5" s="1">
-        <v>95</v>
-      </c>
-      <c r="L5" s="4">
-        <v>7.72</v>
+        <v>16.1904761904762</v>
+      </c>
+      <c r="K5" s="5"/>
+      <c r="L5" s="2">
+        <f t="shared" si="2"/>
+        <v>-0.44000000000000039</v>
       </c>
       <c r="M5" s="1">
-        <v>7.8</v>
+        <f t="shared" si="3"/>
+        <v>-0.36000000000000032</v>
       </c>
       <c r="N5" s="1">
-        <v>8.7048000000000005</v>
-      </c>
-      <c r="O5" s="1">
-        <v>8.8992000000000004</v>
-      </c>
-      <c r="P5" s="3">
-        <v>7.12</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>7.32</v>
-      </c>
+        <f t="shared" si="4"/>
+        <v>-1.04</v>
+      </c>
+      <c r="O5" s="4">
+        <f t="shared" si="5"/>
+        <v>-0.83999999999999986</v>
+      </c>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="2"/>
-    </row>
-    <row r="6" spans="1:20">
+      <c r="S5" s="3"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="2"/>
+    </row>
+    <row r="6" spans="1:23">
       <c r="A6">
         <v>80</v>
       </c>
@@ -84173,53 +84213,56 @@
       <c r="C6" s="1">
         <v>9.1999999999999993</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="8">
         <v>11.68</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="8">
         <v>10.76</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="8">
         <v>10.56</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="7">
+        <v>10.24</v>
+      </c>
+      <c r="H6" s="8">
+        <v>10.4</v>
+      </c>
+      <c r="I6" s="4">
         <f t="shared" si="0"/>
-        <v>16.956521739130441</v>
-      </c>
-      <c r="H6" s="4">
+        <v>11.304347826086968</v>
+      </c>
+      <c r="J6" s="4">
         <f t="shared" si="1"/>
-        <v>14.782608695652188</v>
-      </c>
-      <c r="I6" s="5"/>
-      <c r="J6">
-        <v>80</v>
-      </c>
-      <c r="K6" s="1">
-        <v>119.8</v>
-      </c>
-      <c r="L6" s="1">
-        <v>10.76</v>
-      </c>
-      <c r="M6" s="4">
-        <v>10.56</v>
-      </c>
-      <c r="N6" s="4">
-        <v>12.005999999999997</v>
+        <v>13.043478260869579</v>
+      </c>
+      <c r="K6" s="5"/>
+      <c r="L6" s="2">
+        <f t="shared" si="2"/>
+        <v>-0.91999999999999993</v>
+      </c>
+      <c r="M6" s="1">
+        <f t="shared" si="3"/>
+        <v>-1.1199999999999992</v>
+      </c>
+      <c r="N6" s="1">
+        <f t="shared" si="4"/>
+        <v>-1.4399999999999995</v>
       </c>
       <c r="O6" s="4">
-        <v>12.284799999999997</v>
-      </c>
-      <c r="P6" s="3">
-        <v>10.24</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>10.4</v>
-      </c>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="2"/>
-    </row>
-    <row r="7" spans="1:20">
+        <f t="shared" si="5"/>
+        <v>-1.2799999999999994</v>
+      </c>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="2"/>
+    </row>
+    <row r="7" spans="1:23">
       <c r="A7">
         <v>100</v>
       </c>
@@ -84229,53 +84272,56 @@
       <c r="C7" s="1">
         <v>13.3</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="8">
         <v>16.239999999999998</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="8">
         <v>15.24</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="8">
         <v>14.84</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="7">
+        <v>14.76</v>
+      </c>
+      <c r="H7" s="8">
+        <v>14.84</v>
+      </c>
+      <c r="I7" s="4">
         <f t="shared" si="0"/>
-        <v>14.586466165413528</v>
-      </c>
-      <c r="H7" s="4">
+        <v>10.977443609022549</v>
+      </c>
+      <c r="J7" s="4">
         <f t="shared" si="1"/>
         <v>11.578947368421046</v>
       </c>
-      <c r="I7" s="5"/>
-      <c r="J7">
-        <v>100</v>
-      </c>
-      <c r="K7" s="1">
-        <v>144</v>
-      </c>
-      <c r="L7" s="1">
-        <v>15.24</v>
-      </c>
-      <c r="M7" s="3">
-        <v>14.84</v>
-      </c>
-      <c r="N7" s="4">
-        <v>16.589200000000002</v>
+      <c r="K7" s="5"/>
+      <c r="L7" s="2">
+        <f t="shared" si="2"/>
+        <v>-0.99999999999999822</v>
+      </c>
+      <c r="M7" s="1">
+        <f t="shared" si="3"/>
+        <v>-1.3999999999999986</v>
+      </c>
+      <c r="N7" s="1">
+        <f t="shared" si="4"/>
+        <v>-1.4799999999999986</v>
       </c>
       <c r="O7" s="4">
-        <v>16.943200000000001</v>
-      </c>
-      <c r="P7" s="3">
-        <v>14.76</v>
-      </c>
-      <c r="Q7" s="3">
-        <v>14.84</v>
-      </c>
-      <c r="R7" s="1"/>
+        <f t="shared" si="5"/>
+        <v>-1.3999999999999986</v>
+      </c>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
       <c r="S7" s="3"/>
-      <c r="T7" s="2"/>
-    </row>
-    <row r="8" spans="1:20">
+      <c r="T7" s="3"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="2"/>
+    </row>
+    <row r="8" spans="1:23">
       <c r="A8">
         <v>120</v>
       </c>
@@ -84285,53 +84331,56 @@
       <c r="C8" s="1">
         <v>17.5</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="8">
         <v>20.88</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="8">
         <v>19.920000000000002</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="8">
         <v>19.04</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="7">
+        <v>19</v>
+      </c>
+      <c r="H8" s="8">
+        <v>19.28</v>
+      </c>
+      <c r="I8" s="4">
         <f t="shared" si="0"/>
-        <v>13.828571428571438</v>
-      </c>
-      <c r="H8" s="4">
+        <v>8.5714285714285712</v>
+      </c>
+      <c r="J8" s="4">
         <f t="shared" si="1"/>
-        <v>8.7999999999999954</v>
-      </c>
-      <c r="I8" s="5"/>
-      <c r="J8">
-        <v>120</v>
-      </c>
-      <c r="K8" s="1">
-        <v>168.8</v>
-      </c>
-      <c r="L8" s="1">
-        <v>19.920000000000002</v>
-      </c>
-      <c r="M8" s="3">
-        <v>19.04</v>
-      </c>
-      <c r="N8" s="4">
-        <v>20.982799999999997</v>
+        <v>10.171428571428578</v>
+      </c>
+      <c r="K8" s="5"/>
+      <c r="L8" s="2">
+        <f t="shared" si="2"/>
+        <v>-0.9599999999999973</v>
+      </c>
+      <c r="M8" s="1">
+        <f t="shared" si="3"/>
+        <v>-1.8399999999999999</v>
+      </c>
+      <c r="N8" s="1">
+        <f t="shared" si="4"/>
+        <v>-1.879999999999999</v>
       </c>
       <c r="O8" s="4">
-        <v>21.289199999999997</v>
-      </c>
-      <c r="P8" s="3">
-        <v>19</v>
-      </c>
-      <c r="Q8" s="1">
-        <v>19.28</v>
-      </c>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-      <c r="T8" s="2"/>
-    </row>
-    <row r="9" spans="1:20">
+        <f t="shared" si="5"/>
+        <v>-1.5999999999999979</v>
+      </c>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="2"/>
+    </row>
+    <row r="9" spans="1:23">
       <c r="A9">
         <v>140</v>
       </c>
@@ -84341,53 +84390,56 @@
       <c r="C9" s="1">
         <v>20.9</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="8">
         <v>24.52</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="8">
         <v>23.68</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="8">
         <v>22.96</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="7">
+        <v>22.68</v>
+      </c>
+      <c r="H9" s="8">
+        <v>23.08</v>
+      </c>
+      <c r="I9" s="4">
         <f t="shared" si="0"/>
-        <v>13.30143540669857</v>
-      </c>
-      <c r="H9" s="4">
+        <v>8.5167464114832594</v>
+      </c>
+      <c r="J9" s="4">
         <f t="shared" si="1"/>
-        <v>9.8564593301435526</v>
-      </c>
-      <c r="I9" s="5"/>
-      <c r="J9">
-        <v>140</v>
-      </c>
-      <c r="K9" s="1">
-        <v>193</v>
-      </c>
-      <c r="L9" s="1">
-        <v>23.68</v>
-      </c>
-      <c r="M9" s="4">
-        <v>22.96</v>
-      </c>
-      <c r="N9" s="4">
-        <v>24.921199999999999</v>
+        <v>10.430622009569378</v>
+      </c>
+      <c r="K9" s="5"/>
+      <c r="L9" s="2">
+        <f t="shared" si="2"/>
+        <v>-0.83999999999999986</v>
+      </c>
+      <c r="M9" s="1">
+        <f t="shared" si="3"/>
+        <v>-1.5599999999999987</v>
+      </c>
+      <c r="N9" s="1">
+        <f t="shared" si="4"/>
+        <v>-1.8399999999999999</v>
       </c>
       <c r="O9" s="4">
-        <v>25.280000000000005</v>
-      </c>
-      <c r="P9" s="3">
-        <v>22.68</v>
-      </c>
-      <c r="Q9" s="1">
-        <v>23.08</v>
-      </c>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-      <c r="T9" s="2"/>
-    </row>
-    <row r="10" spans="1:20">
+        <f t="shared" si="5"/>
+        <v>-1.4400000000000013</v>
+      </c>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="2"/>
+    </row>
+    <row r="10" spans="1:23">
       <c r="A10">
         <v>160</v>
       </c>
@@ -84397,53 +84449,56 @@
       <c r="C10" s="1">
         <v>25</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="8">
         <v>29.84</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="8">
         <v>28.28</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="8">
         <v>27.6</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="7">
+        <v>27.24</v>
+      </c>
+      <c r="H10" s="8">
+        <v>27.4</v>
+      </c>
+      <c r="I10" s="4">
         <f t="shared" si="0"/>
-        <v>13.120000000000005</v>
-      </c>
-      <c r="H10" s="4">
+        <v>8.9599999999999937</v>
+      </c>
+      <c r="J10" s="4">
         <f t="shared" si="1"/>
-        <v>10.400000000000006</v>
-      </c>
-      <c r="I10" s="5"/>
-      <c r="J10">
-        <v>160</v>
-      </c>
-      <c r="K10" s="1">
-        <v>217.8</v>
-      </c>
-      <c r="L10" s="1">
-        <v>28.28</v>
-      </c>
-      <c r="M10" s="4">
-        <v>27.6</v>
-      </c>
-      <c r="N10" s="4">
-        <v>29.359600000000004</v>
+        <v>9.5999999999999943</v>
+      </c>
+      <c r="K10" s="5"/>
+      <c r="L10" s="2">
+        <f t="shared" si="2"/>
+        <v>-1.5599999999999987</v>
+      </c>
+      <c r="M10" s="1">
+        <f t="shared" si="3"/>
+        <v>-2.2399999999999984</v>
+      </c>
+      <c r="N10" s="1">
+        <f t="shared" si="4"/>
+        <v>-2.6000000000000014</v>
       </c>
       <c r="O10" s="4">
-        <v>29.831999999999997</v>
-      </c>
-      <c r="P10" s="3">
-        <v>27.24</v>
-      </c>
-      <c r="Q10" s="1">
-        <v>27.4</v>
-      </c>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="2"/>
-    </row>
-    <row r="11" spans="1:20">
+        <f t="shared" si="5"/>
+        <v>-2.4400000000000013</v>
+      </c>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="2"/>
+    </row>
+    <row r="11" spans="1:23">
       <c r="A11">
         <v>180</v>
       </c>
@@ -84453,53 +84508,56 @@
       <c r="C11" s="1">
         <v>29.1</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="8">
         <v>33.44</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="8">
         <v>32.36</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="7">
         <v>31.28</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="7">
+        <v>31.28</v>
+      </c>
+      <c r="H11" s="8">
+        <v>31.76</v>
+      </c>
+      <c r="I11" s="4">
         <f t="shared" si="0"/>
-        <v>11.202749140893463</v>
-      </c>
-      <c r="H11" s="4">
+        <v>7.491408934707902</v>
+      </c>
+      <c r="J11" s="4">
         <f t="shared" si="1"/>
-        <v>7.491408934707902</v>
-      </c>
-      <c r="I11" s="5"/>
-      <c r="J11">
-        <v>180</v>
-      </c>
-      <c r="K11" s="1">
-        <v>242</v>
-      </c>
-      <c r="L11" s="1">
-        <v>32.36</v>
-      </c>
-      <c r="M11" s="3">
-        <v>31.28</v>
-      </c>
-      <c r="N11" s="4">
-        <v>33.793199999999999</v>
+        <v>9.1408934707903775</v>
+      </c>
+      <c r="K11" s="5"/>
+      <c r="L11" s="2">
+        <f t="shared" si="2"/>
+        <v>-1.0799999999999983</v>
+      </c>
+      <c r="M11" s="1">
+        <f t="shared" si="3"/>
+        <v>-2.1599999999999966</v>
+      </c>
+      <c r="N11" s="1">
+        <f t="shared" si="4"/>
+        <v>-2.1599999999999966</v>
       </c>
       <c r="O11" s="4">
-        <v>34.239200000000011</v>
-      </c>
-      <c r="P11" s="3">
-        <v>31.28</v>
-      </c>
-      <c r="Q11" s="1">
-        <v>31.76</v>
-      </c>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
-      <c r="T11" s="2"/>
-    </row>
-    <row r="12" spans="1:20">
+        <f t="shared" si="5"/>
+        <v>-1.6799999999999962</v>
+      </c>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="2"/>
+    </row>
+    <row r="12" spans="1:23">
       <c r="A12">
         <v>200</v>
       </c>
@@ -84509,53 +84567,56 @@
       <c r="C12" s="1">
         <v>32.6</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="8">
         <v>37.56</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="8">
         <v>36</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="7">
         <v>35.200000000000003</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="7">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="H12" s="8">
+        <v>35.4</v>
+      </c>
+      <c r="I12" s="4">
         <f t="shared" si="0"/>
-        <v>10.429447852760731</v>
-      </c>
-      <c r="H12" s="4">
+        <v>7.9754601226993902</v>
+      </c>
+      <c r="J12" s="4">
         <f t="shared" si="1"/>
-        <v>7.9754601226993902</v>
-      </c>
-      <c r="I12" s="5"/>
-      <c r="J12">
-        <v>200</v>
-      </c>
-      <c r="K12" s="1">
-        <v>266.8</v>
-      </c>
-      <c r="L12" s="1">
-        <v>36</v>
-      </c>
-      <c r="M12" s="3">
-        <v>35.200000000000003</v>
-      </c>
-      <c r="N12" s="4">
-        <v>37.643599999999999</v>
+        <v>8.5889570552147152</v>
+      </c>
+      <c r="K12" s="5"/>
+      <c r="L12" s="2">
+        <f t="shared" si="2"/>
+        <v>-1.5600000000000023</v>
+      </c>
+      <c r="M12" s="1">
+        <f t="shared" si="3"/>
+        <v>-2.3599999999999994</v>
+      </c>
+      <c r="N12" s="1">
+        <f t="shared" si="4"/>
+        <v>-2.3599999999999994</v>
       </c>
       <c r="O12" s="4">
-        <v>38.177199999999999</v>
-      </c>
-      <c r="P12" s="3">
-        <v>35.200000000000003</v>
-      </c>
-      <c r="Q12" s="1">
-        <v>35.4</v>
-      </c>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
-      <c r="T12" s="2"/>
-    </row>
-    <row r="13" spans="1:20">
+        <f t="shared" si="5"/>
+        <v>-2.1600000000000037</v>
+      </c>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="2"/>
+    </row>
+    <row r="13" spans="1:23">
       <c r="A13">
         <v>250</v>
       </c>
@@ -84565,53 +84626,56 @@
       <c r="C13" s="1">
         <v>44.6</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="8">
         <v>50.72</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="8">
         <v>48.48</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="7">
         <v>47.76</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="7">
+        <v>47.76</v>
+      </c>
+      <c r="H13" s="8">
+        <v>48</v>
+      </c>
+      <c r="I13" s="4">
         <f t="shared" si="0"/>
-        <v>8.6995515695067169</v>
-      </c>
-      <c r="H13" s="4">
+        <v>7.0852017937219651</v>
+      </c>
+      <c r="J13" s="4">
         <f t="shared" si="1"/>
-        <v>7.0852017937219651</v>
-      </c>
-      <c r="I13" s="5"/>
-      <c r="J13">
-        <v>250</v>
-      </c>
-      <c r="K13" s="1">
-        <v>321</v>
-      </c>
-      <c r="L13" s="1">
-        <v>48.48</v>
-      </c>
-      <c r="M13" s="3">
-        <v>47.76</v>
-      </c>
-      <c r="N13" s="4">
-        <v>50.17</v>
+        <v>7.6233183856502214</v>
+      </c>
+      <c r="K13" s="5"/>
+      <c r="L13" s="2">
+        <f t="shared" si="2"/>
+        <v>-2.240000000000002</v>
+      </c>
+      <c r="M13" s="1">
+        <f t="shared" si="3"/>
+        <v>-2.9600000000000009</v>
+      </c>
+      <c r="N13" s="1">
+        <f t="shared" si="4"/>
+        <v>-2.9600000000000009</v>
       </c>
       <c r="O13" s="4">
-        <v>50.756399999999992</v>
-      </c>
-      <c r="P13" s="3">
-        <v>47.76</v>
-      </c>
-      <c r="Q13" s="1">
-        <v>48</v>
-      </c>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
-      <c r="T13" s="2"/>
-    </row>
-    <row r="14" spans="1:20">
+        <f t="shared" si="5"/>
+        <v>-2.7199999999999989</v>
+      </c>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="2"/>
+    </row>
+    <row r="14" spans="1:23">
       <c r="A14">
         <v>300</v>
       </c>
@@ -84621,53 +84685,56 @@
       <c r="C14" s="1">
         <v>57.4</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="8">
         <v>63.16</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="8">
         <v>61.6</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="8">
         <v>60.84</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="7">
+        <v>60.4</v>
+      </c>
+      <c r="H14" s="8">
+        <v>60.92</v>
+      </c>
+      <c r="I14" s="4">
         <f t="shared" si="0"/>
-        <v>7.317073170731712</v>
-      </c>
-      <c r="H14" s="4">
+        <v>5.2264808362369335</v>
+      </c>
+      <c r="J14" s="4">
         <f t="shared" si="1"/>
-        <v>5.9930313588850259</v>
-      </c>
-      <c r="I14" s="5"/>
-      <c r="J14">
-        <v>300</v>
-      </c>
-      <c r="K14" s="1">
-        <v>380</v>
-      </c>
-      <c r="L14" s="1">
-        <v>61.6</v>
-      </c>
-      <c r="M14" s="4">
-        <v>60.84</v>
-      </c>
-      <c r="N14" s="4">
-        <v>63.017600000000002</v>
+        <v>6.1324041811846746</v>
+      </c>
+      <c r="K14" s="5"/>
+      <c r="L14" s="2">
+        <f t="shared" si="2"/>
+        <v>-1.5599999999999952</v>
+      </c>
+      <c r="M14" s="1">
+        <f t="shared" si="3"/>
+        <v>-2.3199999999999932</v>
+      </c>
+      <c r="N14" s="1">
+        <f t="shared" si="4"/>
+        <v>-2.759999999999998</v>
       </c>
       <c r="O14" s="4">
-        <v>63.494</v>
-      </c>
-      <c r="P14" s="3">
-        <v>60.4</v>
-      </c>
-      <c r="Q14" s="1">
-        <v>60.92</v>
-      </c>
-      <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
-      <c r="T14" s="2"/>
-    </row>
-    <row r="15" spans="1:20">
+        <f t="shared" si="5"/>
+        <v>-2.2399999999999949</v>
+      </c>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="2"/>
+    </row>
+    <row r="15" spans="1:23">
       <c r="A15">
         <v>350</v>
       </c>
@@ -84677,53 +84744,56 @@
       <c r="C15" s="1">
         <v>68.599999999999994</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="8">
         <v>76.12</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="8">
         <v>73.44</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="8">
         <v>72.680000000000007</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="7">
+        <v>72.36</v>
+      </c>
+      <c r="H15" s="8">
+        <v>72.400000000000006</v>
+      </c>
+      <c r="I15" s="4">
         <f t="shared" si="0"/>
-        <v>7.0553935860058372</v>
-      </c>
-      <c r="H15" s="4">
+        <v>5.4810495626822231</v>
+      </c>
+      <c r="J15" s="4">
         <f t="shared" si="1"/>
-        <v>5.9475218658892315</v>
-      </c>
-      <c r="I15" s="5"/>
-      <c r="J15">
-        <v>350</v>
-      </c>
-      <c r="K15" s="1">
-        <v>434.8</v>
-      </c>
-      <c r="L15" s="1">
-        <v>73.44</v>
-      </c>
-      <c r="M15" s="4">
-        <v>72.680000000000007</v>
-      </c>
-      <c r="N15" s="4">
-        <v>75.018800000000013</v>
+        <v>5.5393586005831077</v>
+      </c>
+      <c r="K15" s="5"/>
+      <c r="L15" s="2">
+        <f t="shared" si="2"/>
+        <v>-2.6800000000000068</v>
+      </c>
+      <c r="M15" s="1">
+        <f t="shared" si="3"/>
+        <v>-3.4399999999999977</v>
+      </c>
+      <c r="N15" s="1">
+        <f t="shared" si="4"/>
+        <v>-3.7600000000000051</v>
       </c>
       <c r="O15" s="4">
-        <v>75.558799999999991</v>
-      </c>
-      <c r="P15" s="3">
-        <v>72.36</v>
-      </c>
-      <c r="Q15" s="3">
-        <v>72.400000000000006</v>
-      </c>
-      <c r="R15" s="1"/>
+        <f t="shared" si="5"/>
+        <v>-3.7199999999999989</v>
+      </c>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
       <c r="S15" s="3"/>
-      <c r="T15" s="2"/>
-    </row>
-    <row r="16" spans="1:20">
+      <c r="T15" s="3"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="3"/>
+      <c r="W15" s="2"/>
+    </row>
+    <row r="16" spans="1:23">
       <c r="A16">
         <v>400</v>
       </c>
@@ -84733,53 +84803,56 @@
       <c r="C16" s="1">
         <v>81.8</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="8">
         <v>90.84</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="8">
         <v>87.2</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="8">
         <v>86.52</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="7">
+        <v>85.88</v>
+      </c>
+      <c r="H16" s="8">
+        <v>86.36</v>
+      </c>
+      <c r="I16" s="4">
         <f t="shared" si="0"/>
-        <v>6.6014669926650438</v>
-      </c>
-      <c r="H16" s="4">
+        <v>4.9877750611246929</v>
+      </c>
+      <c r="J16" s="4">
         <f t="shared" si="1"/>
-        <v>5.7701711491442529</v>
-      </c>
-      <c r="I16" s="5"/>
-      <c r="J16">
-        <v>400</v>
-      </c>
-      <c r="K16" s="1">
-        <v>489</v>
-      </c>
-      <c r="L16" s="1">
-        <v>87.2</v>
-      </c>
-      <c r="M16" s="4">
-        <v>86.52</v>
-      </c>
-      <c r="N16" s="4">
-        <v>88.760800000000017</v>
+        <v>5.5745721271393673</v>
+      </c>
+      <c r="K16" s="5"/>
+      <c r="L16" s="2">
+        <f t="shared" si="2"/>
+        <v>-3.6400000000000006</v>
+      </c>
+      <c r="M16" s="1">
+        <f t="shared" si="3"/>
+        <v>-4.3200000000000074</v>
+      </c>
+      <c r="N16" s="1">
+        <f t="shared" si="4"/>
+        <v>-4.960000000000008</v>
       </c>
       <c r="O16" s="4">
-        <v>89.218799999999987</v>
-      </c>
-      <c r="P16" s="3">
-        <v>85.88</v>
-      </c>
-      <c r="Q16" s="1">
-        <v>86.36</v>
-      </c>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-      <c r="T16" s="2"/>
-    </row>
-    <row r="17" spans="1:20">
+        <f t="shared" si="5"/>
+        <v>-4.480000000000004</v>
+      </c>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="2"/>
+    </row>
+    <row r="17" spans="1:23">
       <c r="A17">
         <v>450</v>
       </c>
@@ -84789,53 +84862,56 @@
       <c r="C17" s="1">
         <v>93.4</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="8">
         <v>102.04</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="8">
         <v>98.8</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="8">
         <v>97.84</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="7">
+        <v>97.68</v>
+      </c>
+      <c r="H17" s="8">
+        <v>98.12</v>
+      </c>
+      <c r="I17" s="4">
         <f t="shared" si="0"/>
-        <v>5.7815845824411038</v>
-      </c>
-      <c r="H17" s="4">
+        <v>4.5824411134903649</v>
+      </c>
+      <c r="J17" s="4">
         <f t="shared" si="1"/>
-        <v>4.7537473233404679</v>
-      </c>
-      <c r="I17" s="5"/>
-      <c r="J17">
-        <v>450</v>
-      </c>
-      <c r="K17" s="1">
-        <v>548</v>
-      </c>
-      <c r="L17" s="1">
-        <v>98.8</v>
-      </c>
-      <c r="M17" s="4">
-        <v>97.84</v>
-      </c>
-      <c r="N17" s="4">
-        <v>100.51559999999998</v>
+        <v>5.0535331905781566</v>
+      </c>
+      <c r="K17" s="5"/>
+      <c r="L17" s="2">
+        <f t="shared" si="2"/>
+        <v>-3.2400000000000091</v>
+      </c>
+      <c r="M17" s="1">
+        <f t="shared" si="3"/>
+        <v>-4.2000000000000028</v>
+      </c>
+      <c r="N17" s="1">
+        <f t="shared" si="4"/>
+        <v>-4.3599999999999994</v>
       </c>
       <c r="O17" s="4">
-        <v>101.08880000000001</v>
-      </c>
-      <c r="P17" s="3">
-        <v>97.68</v>
-      </c>
-      <c r="Q17" s="1">
-        <v>98.12</v>
-      </c>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-      <c r="T17" s="2"/>
-    </row>
-    <row r="18" spans="1:20">
+        <f t="shared" si="5"/>
+        <v>-3.9200000000000017</v>
+      </c>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="2"/>
+    </row>
+    <row r="18" spans="1:23">
       <c r="A18">
         <v>500</v>
       </c>
@@ -84845,51 +84921,141 @@
       <c r="C18" s="1">
         <v>106.7</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="8">
         <v>116.64</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="8">
         <v>112.68</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="8">
         <v>111.28</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="7">
+        <v>111</v>
+      </c>
+      <c r="H18" s="8">
+        <v>111.8</v>
+      </c>
+      <c r="I18" s="4">
         <f t="shared" si="0"/>
-        <v>5.6044985941893195</v>
-      </c>
-      <c r="H18" s="4">
+        <v>4.0299906279287692</v>
+      </c>
+      <c r="J18" s="4">
         <f t="shared" si="1"/>
-        <v>4.292408622305528</v>
-      </c>
-      <c r="I18" s="1"/>
-      <c r="J18">
-        <v>500</v>
-      </c>
-      <c r="K18" s="1">
-        <v>602.79999999999995</v>
-      </c>
-      <c r="L18" s="1">
-        <v>112.68</v>
-      </c>
-      <c r="M18" s="4">
-        <v>111.28</v>
-      </c>
-      <c r="N18" s="4">
-        <v>114.05479999999997</v>
+        <v>4.7797563261480738</v>
+      </c>
+      <c r="K18" s="1"/>
+      <c r="L18" s="2">
+        <f t="shared" si="2"/>
+        <v>-3.9599999999999937</v>
+      </c>
+      <c r="M18" s="1">
+        <f t="shared" si="3"/>
+        <v>-5.3599999999999994</v>
+      </c>
+      <c r="N18" s="1">
+        <f t="shared" si="4"/>
+        <v>-5.6400000000000006</v>
       </c>
       <c r="O18" s="4">
-        <v>114.58679999999995</v>
-      </c>
-      <c r="P18" s="3">
-        <v>111</v>
-      </c>
-      <c r="Q18" s="1">
-        <v>111.8</v>
-      </c>
-      <c r="R18" s="1"/>
-      <c r="S18" s="1"/>
-      <c r="T18" s="2"/>
+        <f t="shared" si="5"/>
+        <v>-4.8400000000000034</v>
+      </c>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="3"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="2"/>
+    </row>
+    <row r="19" spans="1:23">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="3"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="2"/>
+    </row>
+    <row r="20" spans="1:23">
+      <c r="K20" t="s">
+        <v>564</v>
+      </c>
+      <c r="L20" s="2">
+        <f>COUNTIF(L3:L18,"&lt;0")</f>
+        <v>14</v>
+      </c>
+      <c r="M20" s="1">
+        <f>COUNTIF(M3:M18,"&lt;0")</f>
+        <v>15</v>
+      </c>
+      <c r="N20" s="1">
+        <f t="shared" ref="N20:O20" si="6">COUNTIF(N3:N18,"&lt;0")</f>
+        <v>16</v>
+      </c>
+      <c r="O20" s="1">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23">
+      <c r="K21" t="s">
+        <v>565</v>
+      </c>
+      <c r="L21" s="2">
+        <f>COUNTIF(L3:L18,"&gt;0")</f>
+        <v>2</v>
+      </c>
+      <c r="M21" s="1">
+        <f>COUNTIF(M3:M18,"&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="N21" s="1">
+        <f t="shared" ref="N21:O21" si="7">COUNTIF(N3:N18,"&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="O21" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23">
+      <c r="K22" t="s">
+        <v>566</v>
+      </c>
+      <c r="L22">
+        <f>COUNTIF(L3:L18,"=0")</f>
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <f>COUNTIF(M3:M18,"=0")</f>
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <f t="shared" ref="N22:O22" si="8">COUNTIF(N3:N18,"=0")</f>
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -84899,31 +85065,39 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V27"/>
+  <dimension ref="A1:X31"/>
   <sheetViews>
-    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:R1048576"/>
+    <sheetView zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:24">
       <c r="A1" t="s">
         <v>549</v>
       </c>
-      <c r="K1" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22">
+    </row>
+    <row r="2" spans="1:24">
       <c r="A2" s="5" t="s">
         <v>545</v>
       </c>
@@ -84943,41 +85117,39 @@
         <v>4</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>550</v>
+        <v>560</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>551</v>
-      </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5" t="s">
-        <v>545</v>
-      </c>
+        <v>561</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>558</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>559</v>
+      </c>
+      <c r="K2" s="5"/>
       <c r="L2" s="5" t="s">
-        <v>546</v>
+        <v>562</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>2</v>
+        <v>563</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>4</v>
+        <v>567</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>554</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>558</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>552</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>553</v>
-      </c>
+        <v>568</v>
+      </c>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
-    </row>
-    <row r="3" spans="1:22">
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+    </row>
+    <row r="3" spans="1:24">
       <c r="A3">
         <v>600</v>
       </c>
@@ -84990,52 +85162,54 @@
       <c r="D3" s="1">
         <v>187.6</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="4">
         <v>185.4</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="4">
         <v>185.6</v>
       </c>
-      <c r="G3" s="1">
-        <f>(E3-C3)/C3*100</f>
-        <v>0.87051142546245608</v>
-      </c>
-      <c r="H3" s="1">
-        <f>(F3-C3)/C3*100</f>
-        <v>0.9793253536452573</v>
-      </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3">
-        <v>600</v>
-      </c>
-      <c r="L3">
-        <v>637</v>
-      </c>
-      <c r="M3" s="3">
-        <v>185.4</v>
+      <c r="G3" s="3">
+        <v>184.6</v>
+      </c>
+      <c r="H3" s="3">
+        <v>184.6</v>
+      </c>
+      <c r="I3" s="1">
+        <f>(G3-C3)/C3*100</f>
+        <v>0.43525571273122032</v>
+      </c>
+      <c r="J3" s="1">
+        <f>(H3-C3)/C3*100</f>
+        <v>0.43525571273122032</v>
+      </c>
+      <c r="K3" s="1"/>
+      <c r="L3" s="2">
+        <f>E3-D3</f>
+        <v>-2.1999999999999886</v>
+      </c>
+      <c r="M3" s="1">
+        <f>F3-D3</f>
+        <v>-2</v>
       </c>
       <c r="N3" s="1">
-        <v>185.6</v>
-      </c>
-      <c r="O3" s="1">
-        <v>186.07</v>
-      </c>
-      <c r="P3" s="1">
-        <v>185.85</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>184.6</v>
-      </c>
-      <c r="R3" s="1">
-        <v>184.6</v>
-      </c>
+        <f>G3-D3</f>
+        <v>-3</v>
+      </c>
+      <c r="O3" s="4">
+        <f>H3-D3</f>
+        <v>-3</v>
+      </c>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-    </row>
-    <row r="4" spans="1:22">
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+    </row>
+    <row r="4" spans="1:24">
       <c r="A4">
         <v>600</v>
       </c>
@@ -85048,52 +85222,54 @@
       <c r="D4" s="1">
         <v>173.4</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="4">
         <v>171.4</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="4">
         <v>171</v>
       </c>
-      <c r="G4" s="1">
-        <f t="shared" ref="G4:G27" si="0">(E4-C4)/C4*100</f>
-        <v>2.5119617224880484</v>
-      </c>
-      <c r="H4" s="1">
-        <f t="shared" ref="H4:H27" si="1">(F4-C4)/C4*100</f>
-        <v>2.2727272727272796</v>
-      </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4">
-        <v>600</v>
-      </c>
-      <c r="L4">
-        <v>674</v>
+      <c r="G4" s="4">
+        <v>170.2</v>
+      </c>
+      <c r="H4" s="3">
+        <v>170</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" ref="I4:I27" si="0">(G4-C4)/C4*100</f>
+        <v>1.7942583732057416</v>
+      </c>
+      <c r="J4" s="1">
+        <f t="shared" ref="J4:J27" si="1">(H4-C4)/C4*100</f>
+        <v>1.6746411483253658</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="2">
+        <f t="shared" ref="L4:L27" si="2">E4-D4</f>
+        <v>-2</v>
       </c>
       <c r="M4" s="1">
-        <v>171.4</v>
-      </c>
-      <c r="N4" s="3">
-        <v>171</v>
-      </c>
-      <c r="O4" s="1">
-        <v>171.15199999999999</v>
-      </c>
-      <c r="P4" s="1">
-        <v>171.24</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>170.2</v>
-      </c>
-      <c r="R4" s="3">
-        <v>170</v>
-      </c>
+        <f t="shared" ref="M4:M27" si="3">F4-D4</f>
+        <v>-2.4000000000000057</v>
+      </c>
+      <c r="N4" s="1">
+        <f t="shared" ref="N4:N27" si="4">G4-D4</f>
+        <v>-3.2000000000000171</v>
+      </c>
+      <c r="O4" s="4">
+        <f t="shared" ref="O4:O27" si="5">H4-D4</f>
+        <v>-3.4000000000000057</v>
+      </c>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
       <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-    </row>
-    <row r="5" spans="1:22">
+      <c r="T4" s="3"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+    </row>
+    <row r="5" spans="1:24">
       <c r="A5">
         <v>600</v>
       </c>
@@ -85106,52 +85282,54 @@
       <c r="D5" s="1">
         <v>159.4</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="4">
         <v>156.19999999999999</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="4">
         <v>156.6</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="3">
+        <v>154</v>
+      </c>
+      <c r="H5" s="4">
+        <v>154.19999999999999</v>
+      </c>
+      <c r="I5" s="1">
         <f t="shared" si="0"/>
-        <v>3.7184594953519223</v>
-      </c>
-      <c r="H5" s="1">
+        <v>2.2576361221779586</v>
+      </c>
+      <c r="J5" s="1">
         <f t="shared" si="1"/>
-        <v>3.9840637450199203</v>
-      </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5">
-        <v>600</v>
-      </c>
-      <c r="L5">
-        <v>712</v>
-      </c>
-      <c r="M5" s="3">
-        <v>156.19999999999999</v>
+        <v>2.3904382470119487</v>
+      </c>
+      <c r="K5" s="1"/>
+      <c r="L5" s="2">
+        <f t="shared" si="2"/>
+        <v>-3.2000000000000171</v>
+      </c>
+      <c r="M5" s="1">
+        <f t="shared" si="3"/>
+        <v>-2.8000000000000114</v>
       </c>
       <c r="N5" s="1">
-        <v>156.6</v>
-      </c>
-      <c r="O5" s="1">
-        <v>156.33599999999998</v>
-      </c>
-      <c r="P5" s="1">
-        <v>156.566</v>
-      </c>
-      <c r="Q5" s="3">
-        <v>154</v>
-      </c>
-      <c r="R5" s="1">
-        <v>154.19999999999999</v>
-      </c>
-      <c r="S5" s="1"/>
+        <f t="shared" si="4"/>
+        <v>-5.4000000000000057</v>
+      </c>
+      <c r="O5" s="4">
+        <f t="shared" si="5"/>
+        <v>-5.2000000000000171</v>
+      </c>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="3"/>
       <c r="T5" s="1"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
-    </row>
-    <row r="6" spans="1:22">
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+    </row>
+    <row r="6" spans="1:24">
       <c r="A6">
         <v>600</v>
       </c>
@@ -85164,52 +85342,54 @@
       <c r="D6" s="1">
         <v>145.4</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="4">
         <v>145.6</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="4">
         <v>144.4</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="3">
+        <v>142.6</v>
+      </c>
+      <c r="H6" s="4">
+        <v>143.19999999999999</v>
+      </c>
+      <c r="I6" s="1">
         <f t="shared" si="0"/>
-        <v>4.8991354466858663</v>
-      </c>
-      <c r="H6" s="1">
+        <v>2.7377521613832729</v>
+      </c>
+      <c r="J6" s="1">
         <f t="shared" si="1"/>
-        <v>4.0345821325648377</v>
-      </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6">
-        <v>600</v>
-      </c>
-      <c r="L6">
-        <v>749</v>
+        <v>3.1700288184437877</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="L6" s="2">
+        <f>E6-D6</f>
+        <v>0.19999999999998863</v>
       </c>
       <c r="M6" s="1">
-        <v>145.6</v>
-      </c>
-      <c r="N6" s="3">
-        <v>144.4</v>
-      </c>
-      <c r="O6" s="1">
-        <v>145.19400000000002</v>
-      </c>
-      <c r="P6" s="1">
-        <v>145.30400000000003</v>
-      </c>
-      <c r="Q6" s="3">
-        <v>142.6</v>
-      </c>
-      <c r="R6" s="1">
-        <v>143.19999999999999</v>
-      </c>
-      <c r="S6" s="1"/>
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="N6" s="1">
+        <f t="shared" si="4"/>
+        <v>-2.8000000000000114</v>
+      </c>
+      <c r="O6" s="4">
+        <f t="shared" si="5"/>
+        <v>-2.2000000000000171</v>
+      </c>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="3"/>
       <c r="T6" s="1"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
-    </row>
-    <row r="7" spans="1:22">
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+    </row>
+    <row r="7" spans="1:24">
       <c r="A7">
         <v>600</v>
       </c>
@@ -85222,52 +85402,54 @@
       <c r="D7" s="1">
         <v>135.4</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="4">
         <v>133.80000000000001</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="4">
         <v>133.80000000000001</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="3">
+        <v>131.6</v>
+      </c>
+      <c r="H7" s="4">
+        <v>132</v>
+      </c>
+      <c r="I7" s="1">
         <f t="shared" si="0"/>
-        <v>6.3593004769475474</v>
-      </c>
-      <c r="H7" s="1">
+        <v>4.6104928457869612</v>
+      </c>
+      <c r="J7" s="1">
         <f t="shared" si="1"/>
-        <v>6.3593004769475474</v>
-      </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7">
-        <v>600</v>
-      </c>
-      <c r="L7">
-        <v>787</v>
-      </c>
-      <c r="M7" s="3">
-        <v>133.80000000000001</v>
-      </c>
-      <c r="N7" s="3">
-        <v>133.80000000000001</v>
-      </c>
-      <c r="O7" s="1">
-        <v>133.99399999999997</v>
-      </c>
-      <c r="P7" s="1">
-        <v>134.458</v>
-      </c>
-      <c r="Q7" s="3">
-        <v>131.6</v>
-      </c>
-      <c r="R7" s="1">
-        <v>132</v>
-      </c>
-      <c r="S7" s="1"/>
+        <v>4.9284578696343422</v>
+      </c>
+      <c r="K7" s="1"/>
+      <c r="L7" s="2">
+        <f t="shared" si="2"/>
+        <v>-1.5999999999999943</v>
+      </c>
+      <c r="M7" s="1">
+        <f t="shared" si="3"/>
+        <v>-1.5999999999999943</v>
+      </c>
+      <c r="N7" s="1">
+        <f t="shared" si="4"/>
+        <v>-3.8000000000000114</v>
+      </c>
+      <c r="O7" s="4">
+        <f t="shared" si="5"/>
+        <v>-3.4000000000000057</v>
+      </c>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="3"/>
       <c r="T7" s="1"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
-    </row>
-    <row r="8" spans="1:22">
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+    </row>
+    <row r="8" spans="1:24">
       <c r="A8">
         <v>700</v>
       </c>
@@ -85280,52 +85462,54 @@
       <c r="D8" s="1">
         <v>218.8</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="4">
         <v>217</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="4">
         <v>217.2</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="3">
+        <v>216.2</v>
+      </c>
+      <c r="H8" s="3">
+        <v>216.2</v>
+      </c>
+      <c r="I8" s="1">
         <f t="shared" si="0"/>
-        <v>1.2126865671641764</v>
-      </c>
-      <c r="H8" s="1">
+        <v>0.83955223880596219</v>
+      </c>
+      <c r="J8" s="1">
         <f t="shared" si="1"/>
-        <v>1.3059701492537232</v>
-      </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8">
-        <v>700</v>
-      </c>
-      <c r="L8">
-        <v>740</v>
-      </c>
-      <c r="M8" s="3">
-        <v>217</v>
+        <v>0.83955223880596219</v>
+      </c>
+      <c r="K8" s="1"/>
+      <c r="L8" s="2">
+        <f t="shared" si="2"/>
+        <v>-1.8000000000000114</v>
+      </c>
+      <c r="M8" s="1">
+        <f t="shared" si="3"/>
+        <v>-1.6000000000000227</v>
       </c>
       <c r="N8" s="1">
-        <v>217.2</v>
-      </c>
-      <c r="O8" s="1">
-        <v>217.29000000000002</v>
-      </c>
-      <c r="P8" s="1">
-        <v>217.27799999999996</v>
-      </c>
-      <c r="Q8" s="3">
-        <v>216.2</v>
-      </c>
-      <c r="R8" s="3">
-        <v>216.2</v>
-      </c>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
-      <c r="U8" s="2"/>
-      <c r="V8" s="2"/>
-    </row>
-    <row r="9" spans="1:22">
+        <f t="shared" si="4"/>
+        <v>-2.6000000000000227</v>
+      </c>
+      <c r="O8" s="4">
+        <f t="shared" si="5"/>
+        <v>-2.6000000000000227</v>
+      </c>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+    </row>
+    <row r="9" spans="1:24">
       <c r="A9">
         <v>700</v>
       </c>
@@ -85338,52 +85522,54 @@
       <c r="D9" s="1">
         <v>204.4</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="4">
         <v>202.6</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="4">
         <v>202</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="3">
+        <v>201</v>
+      </c>
+      <c r="H9" s="3">
+        <v>201</v>
+      </c>
+      <c r="I9" s="1">
         <f t="shared" si="0"/>
-        <v>2.3232323232323204</v>
-      </c>
-      <c r="H9" s="1">
+        <v>1.5151515151515151</v>
+      </c>
+      <c r="J9" s="1">
         <f t="shared" si="1"/>
-        <v>2.0202020202020203</v>
-      </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9">
-        <v>700</v>
-      </c>
-      <c r="L9">
-        <v>780</v>
+        <v>1.5151515151515151</v>
+      </c>
+      <c r="K9" s="1"/>
+      <c r="L9" s="2">
+        <f t="shared" si="2"/>
+        <v>-1.8000000000000114</v>
       </c>
       <c r="M9" s="1">
-        <v>202.6</v>
-      </c>
-      <c r="N9" s="3">
-        <v>202</v>
-      </c>
-      <c r="O9" s="1">
-        <v>202.51600000000002</v>
-      </c>
-      <c r="P9" s="1">
-        <v>202.64600000000002</v>
-      </c>
-      <c r="Q9" s="3">
-        <v>201</v>
-      </c>
-      <c r="R9" s="3">
-        <v>201</v>
-      </c>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="2"/>
-      <c r="V9" s="2"/>
-    </row>
-    <row r="10" spans="1:22">
+        <f t="shared" si="3"/>
+        <v>-2.4000000000000057</v>
+      </c>
+      <c r="N9" s="1">
+        <f t="shared" si="4"/>
+        <v>-3.4000000000000057</v>
+      </c>
+      <c r="O9" s="4">
+        <f t="shared" si="5"/>
+        <v>-3.4000000000000057</v>
+      </c>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+    </row>
+    <row r="10" spans="1:24">
       <c r="A10">
         <v>700</v>
       </c>
@@ -85396,52 +85582,54 @@
       <c r="D10" s="1">
         <v>189</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="4">
         <v>185.6</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="4">
         <v>185.8</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="3">
+        <v>184</v>
+      </c>
+      <c r="H10" s="3">
+        <v>184</v>
+      </c>
+      <c r="I10" s="1">
         <f t="shared" si="0"/>
-        <v>3.1111111111111081</v>
-      </c>
-      <c r="H10" s="1">
+        <v>2.2222222222222223</v>
+      </c>
+      <c r="J10" s="1">
         <f t="shared" si="1"/>
-        <v>3.2222222222222285</v>
-      </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10">
-        <v>700</v>
-      </c>
-      <c r="L10">
-        <v>821</v>
-      </c>
-      <c r="M10" s="3">
-        <v>185.6</v>
+        <v>2.2222222222222223</v>
+      </c>
+      <c r="K10" s="1"/>
+      <c r="L10" s="2">
+        <f t="shared" si="2"/>
+        <v>-3.4000000000000057</v>
+      </c>
+      <c r="M10" s="1">
+        <f t="shared" si="3"/>
+        <v>-3.1999999999999886</v>
       </c>
       <c r="N10" s="1">
-        <v>185.8</v>
-      </c>
-      <c r="O10" s="1">
-        <v>185.79599999999999</v>
-      </c>
-      <c r="P10" s="1">
-        <v>185.77</v>
-      </c>
-      <c r="Q10" s="3">
-        <v>184</v>
-      </c>
-      <c r="R10" s="3">
-        <v>184</v>
-      </c>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="2"/>
-      <c r="V10" s="2"/>
-    </row>
-    <row r="11" spans="1:22" ht="13.5" customHeight="1">
+        <f t="shared" si="4"/>
+        <v>-5</v>
+      </c>
+      <c r="O10" s="4">
+        <f t="shared" si="5"/>
+        <v>-5</v>
+      </c>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+    </row>
+    <row r="11" spans="1:24" ht="13.5" customHeight="1">
       <c r="A11">
         <v>700</v>
       </c>
@@ -85454,52 +85642,54 @@
       <c r="D11" s="1">
         <v>174.2</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="4">
         <v>171.4</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="4">
         <v>170.8</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="4">
+        <v>168.8</v>
+      </c>
+      <c r="H11" s="3">
+        <v>168.6</v>
+      </c>
+      <c r="I11" s="1">
         <f t="shared" si="0"/>
-        <v>4.5121951219512226</v>
-      </c>
-      <c r="H11" s="1">
+        <v>2.9268292682926895</v>
+      </c>
+      <c r="J11" s="1">
         <f t="shared" si="1"/>
-        <v>4.1463414634146414</v>
-      </c>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11">
-        <v>700</v>
-      </c>
-      <c r="L11">
-        <v>861</v>
+        <v>2.8048780487804845</v>
+      </c>
+      <c r="K11" s="1"/>
+      <c r="L11" s="2">
+        <f t="shared" si="2"/>
+        <v>-2.7999999999999829</v>
       </c>
       <c r="M11" s="1">
-        <v>171.4</v>
-      </c>
-      <c r="N11" s="3">
-        <v>170.8</v>
-      </c>
-      <c r="O11" s="1">
-        <v>171.226</v>
-      </c>
-      <c r="P11" s="1">
-        <v>171.24799999999999</v>
-      </c>
-      <c r="Q11" s="1">
-        <v>168.8</v>
-      </c>
-      <c r="R11" s="3">
-        <v>168.6</v>
-      </c>
+        <f t="shared" si="3"/>
+        <v>-3.3999999999999773</v>
+      </c>
+      <c r="N11" s="1">
+        <f t="shared" si="4"/>
+        <v>-5.3999999999999773</v>
+      </c>
+      <c r="O11" s="4">
+        <f t="shared" si="5"/>
+        <v>-5.5999999999999943</v>
+      </c>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
       <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
-      <c r="U11" s="2"/>
-      <c r="V11" s="2"/>
-    </row>
-    <row r="12" spans="1:22">
+      <c r="T11" s="3"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+    </row>
+    <row r="12" spans="1:24">
       <c r="A12">
         <v>700</v>
       </c>
@@ -85512,52 +85702,54 @@
       <c r="D12" s="1">
         <v>165.2</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="4">
         <v>161.80000000000001</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="4">
         <v>162.19999999999999</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="3">
+        <v>159</v>
+      </c>
+      <c r="H12" s="4">
+        <v>159.6</v>
+      </c>
+      <c r="I12" s="1">
         <f t="shared" si="0"/>
-        <v>4.9286640726329596</v>
-      </c>
-      <c r="H12" s="1">
+        <v>3.1128404669260776</v>
+      </c>
+      <c r="J12" s="1">
         <f t="shared" si="1"/>
-        <v>5.1880674448767836</v>
-      </c>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12">
-        <v>700</v>
-      </c>
-      <c r="L12">
-        <v>902</v>
-      </c>
-      <c r="M12" s="3">
-        <v>161.80000000000001</v>
+        <v>3.5019455252918332</v>
+      </c>
+      <c r="K12" s="1"/>
+      <c r="L12" s="2">
+        <f t="shared" si="2"/>
+        <v>-3.3999999999999773</v>
+      </c>
+      <c r="M12" s="1">
+        <f t="shared" si="3"/>
+        <v>-3</v>
       </c>
       <c r="N12" s="1">
-        <v>162.19999999999999</v>
-      </c>
-      <c r="O12" s="1">
-        <v>162.28800000000001</v>
-      </c>
-      <c r="P12" s="1">
-        <v>162.65199999999999</v>
-      </c>
-      <c r="Q12" s="3">
-        <v>159</v>
-      </c>
-      <c r="R12" s="1">
-        <v>159.6</v>
-      </c>
-      <c r="S12" s="1"/>
+        <f t="shared" si="4"/>
+        <v>-6.1999999999999886</v>
+      </c>
+      <c r="O12" s="4">
+        <f t="shared" si="5"/>
+        <v>-5.5999999999999943</v>
+      </c>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="3"/>
       <c r="T12" s="1"/>
-      <c r="U12" s="2"/>
-      <c r="V12" s="2"/>
-    </row>
-    <row r="13" spans="1:22">
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+    </row>
+    <row r="13" spans="1:24">
       <c r="A13">
         <v>800</v>
       </c>
@@ -85570,52 +85762,54 @@
       <c r="D13" s="1">
         <v>250.8</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="4">
         <v>248.4</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="4">
         <v>248.8</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="3">
+        <v>247.8</v>
+      </c>
+      <c r="H13" s="3">
+        <v>247.8</v>
+      </c>
+      <c r="I13" s="1">
         <f t="shared" si="0"/>
-        <v>1.1400651465798093</v>
-      </c>
-      <c r="H13" s="1">
+        <v>0.89576547231271053</v>
+      </c>
+      <c r="J13" s="1">
         <f t="shared" si="1"/>
-        <v>1.3029315960912122</v>
-      </c>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13">
-        <v>800</v>
-      </c>
-      <c r="L13">
-        <v>843</v>
-      </c>
-      <c r="M13" s="3">
-        <v>248.4</v>
+        <v>0.89576547231271053</v>
+      </c>
+      <c r="K13" s="1"/>
+      <c r="L13" s="2">
+        <f t="shared" si="2"/>
+        <v>-2.4000000000000057</v>
+      </c>
+      <c r="M13" s="1">
+        <f t="shared" si="3"/>
+        <v>-2</v>
       </c>
       <c r="N13" s="1">
-        <v>248.8</v>
-      </c>
-      <c r="O13" s="1">
-        <v>248.50399999999999</v>
-      </c>
-      <c r="P13" s="1">
-        <v>248.58</v>
-      </c>
-      <c r="Q13" s="3">
-        <v>247.8</v>
-      </c>
-      <c r="R13" s="3">
-        <v>247.8</v>
-      </c>
-      <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
-      <c r="U13" s="2"/>
-      <c r="V13" s="2"/>
-    </row>
-    <row r="14" spans="1:22">
+        <f t="shared" si="4"/>
+        <v>-3</v>
+      </c>
+      <c r="O13" s="4">
+        <f t="shared" si="5"/>
+        <v>-3</v>
+      </c>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+    </row>
+    <row r="14" spans="1:24">
       <c r="A14">
         <v>800</v>
       </c>
@@ -85628,52 +85822,54 @@
       <c r="D14" s="1">
         <v>235</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="4">
         <v>232</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="4">
         <v>231.8</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="3">
+        <v>230.6</v>
+      </c>
+      <c r="H14" s="3">
+        <v>230.6</v>
+      </c>
+      <c r="I14" s="1">
         <f t="shared" si="0"/>
-        <v>1.9332161687170502</v>
-      </c>
-      <c r="H14" s="1">
+        <v>1.3181019332161688</v>
+      </c>
+      <c r="J14" s="1">
         <f t="shared" si="1"/>
-        <v>1.8453427065026438</v>
-      </c>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14">
-        <v>800</v>
-      </c>
-      <c r="L14">
-        <v>886</v>
+        <v>1.3181019332161688</v>
+      </c>
+      <c r="K14" s="1"/>
+      <c r="L14" s="2">
+        <f t="shared" si="2"/>
+        <v>-3</v>
       </c>
       <c r="M14" s="1">
-        <v>232</v>
-      </c>
-      <c r="N14" s="3">
-        <v>231.8</v>
-      </c>
-      <c r="O14" s="1">
-        <v>231.92600000000002</v>
-      </c>
-      <c r="P14" s="1">
-        <v>231.92399999999998</v>
-      </c>
-      <c r="Q14" s="3">
-        <v>230.6</v>
-      </c>
-      <c r="R14" s="3">
-        <v>230.6</v>
-      </c>
-      <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
-      <c r="U14" s="2"/>
-      <c r="V14" s="2"/>
-    </row>
-    <row r="15" spans="1:22" ht="14.25" customHeight="1">
+        <f t="shared" si="3"/>
+        <v>-3.1999999999999886</v>
+      </c>
+      <c r="N14" s="1">
+        <f t="shared" si="4"/>
+        <v>-4.4000000000000057</v>
+      </c>
+      <c r="O14" s="4">
+        <f t="shared" si="5"/>
+        <v>-4.4000000000000057</v>
+      </c>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+    </row>
+    <row r="15" spans="1:24" ht="14.25" customHeight="1">
       <c r="A15">
         <v>800</v>
       </c>
@@ -85686,52 +85882,54 @@
       <c r="D15" s="1">
         <v>216.2</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="4">
         <v>215.2</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="4">
         <v>215.2</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="3">
+        <v>212.6</v>
+      </c>
+      <c r="H15" s="4">
+        <v>213.2</v>
+      </c>
+      <c r="I15" s="1">
         <f t="shared" si="0"/>
-        <v>3.2629558541266714</v>
-      </c>
-      <c r="H15" s="1">
+        <v>2.0153550863723555</v>
+      </c>
+      <c r="J15" s="1">
         <f t="shared" si="1"/>
-        <v>3.2629558541266714</v>
-      </c>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15">
-        <v>800</v>
-      </c>
-      <c r="L15">
-        <v>930</v>
-      </c>
-      <c r="M15" s="3">
-        <v>215.2</v>
-      </c>
-      <c r="N15" s="3">
-        <v>215.2</v>
-      </c>
-      <c r="O15" s="1">
-        <v>214.86799999999999</v>
-      </c>
-      <c r="P15" s="1">
-        <v>214.87800000000001</v>
-      </c>
-      <c r="Q15" s="3">
-        <v>212.6</v>
-      </c>
-      <c r="R15" s="1">
-        <v>213.2</v>
-      </c>
-      <c r="S15" s="1"/>
+        <v>2.3032629558541187</v>
+      </c>
+      <c r="K15" s="1"/>
+      <c r="L15" s="2">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="M15" s="1">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="N15" s="1">
+        <f t="shared" si="4"/>
+        <v>-3.5999999999999943</v>
+      </c>
+      <c r="O15" s="4">
+        <f t="shared" si="5"/>
+        <v>-3</v>
+      </c>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="3"/>
       <c r="T15" s="1"/>
-      <c r="U15" s="2"/>
-      <c r="V15" s="2"/>
-    </row>
-    <row r="16" spans="1:22">
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+    </row>
+    <row r="16" spans="1:24">
       <c r="A16">
         <v>800</v>
       </c>
@@ -85744,52 +85942,54 @@
       <c r="D16" s="1">
         <v>205</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="4">
         <v>201.6</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="4">
         <v>200.6</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="3">
+        <v>198.8</v>
+      </c>
+      <c r="H16" s="4">
+        <v>199</v>
+      </c>
+      <c r="I16" s="1">
         <f t="shared" si="0"/>
-        <v>3.8105046343975317</v>
-      </c>
-      <c r="H16" s="1">
+        <v>2.368692070030908</v>
+      </c>
+      <c r="J16" s="1">
         <f t="shared" si="1"/>
-        <v>3.2955715756951629</v>
-      </c>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16">
-        <v>800</v>
-      </c>
-      <c r="L16">
-        <v>973</v>
+        <v>2.4716786817713761</v>
+      </c>
+      <c r="K16" s="1"/>
+      <c r="L16" s="2">
+        <f t="shared" si="2"/>
+        <v>-3.4000000000000057</v>
       </c>
       <c r="M16" s="1">
-        <v>201.6</v>
-      </c>
-      <c r="N16" s="3">
-        <v>200.6</v>
-      </c>
-      <c r="O16" s="1">
-        <v>201.42000000000002</v>
-      </c>
-      <c r="P16" s="1">
-        <v>201.49600000000001</v>
-      </c>
-      <c r="Q16" s="3">
-        <v>198.8</v>
-      </c>
-      <c r="R16" s="1">
-        <v>199</v>
-      </c>
-      <c r="S16" s="1"/>
+        <f t="shared" si="3"/>
+        <v>-4.4000000000000057</v>
+      </c>
+      <c r="N16" s="1">
+        <f t="shared" si="4"/>
+        <v>-6.1999999999999886</v>
+      </c>
+      <c r="O16" s="4">
+        <f t="shared" si="5"/>
+        <v>-6</v>
+      </c>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="3"/>
       <c r="T16" s="1"/>
-      <c r="U16" s="2"/>
-      <c r="V16" s="2"/>
-    </row>
-    <row r="17" spans="1:22">
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+    </row>
+    <row r="17" spans="1:24">
       <c r="A17">
         <v>800</v>
       </c>
@@ -85802,52 +86002,54 @@
       <c r="D17" s="1">
         <v>189</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="4">
         <v>184.8</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="4">
         <v>184.4</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17" s="3">
+        <v>182.6</v>
+      </c>
+      <c r="H17" s="4">
+        <v>182.8</v>
+      </c>
+      <c r="I17" s="1">
         <f t="shared" si="0"/>
-        <v>4.8808172531214655</v>
-      </c>
-      <c r="H17" s="1">
+        <v>3.632236095346201</v>
+      </c>
+      <c r="J17" s="1">
         <f t="shared" si="1"/>
-        <v>4.6538024971623262</v>
-      </c>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17">
-        <v>800</v>
-      </c>
-      <c r="L17">
-        <v>1017</v>
+        <v>3.7457434733257791</v>
+      </c>
+      <c r="K17" s="1"/>
+      <c r="L17" s="2">
+        <f t="shared" si="2"/>
+        <v>-4.1999999999999886</v>
       </c>
       <c r="M17" s="1">
-        <v>184.8</v>
-      </c>
-      <c r="N17" s="3">
-        <v>184.4</v>
-      </c>
-      <c r="O17" s="1">
-        <v>185.44199999999998</v>
-      </c>
-      <c r="P17" s="1">
-        <v>185.744</v>
-      </c>
-      <c r="Q17" s="3">
-        <v>182.6</v>
-      </c>
-      <c r="R17" s="1">
-        <v>182.8</v>
-      </c>
-      <c r="S17" s="1"/>
+        <f t="shared" si="3"/>
+        <v>-4.5999999999999943</v>
+      </c>
+      <c r="N17" s="1">
+        <f t="shared" si="4"/>
+        <v>-6.4000000000000057</v>
+      </c>
+      <c r="O17" s="4">
+        <f t="shared" si="5"/>
+        <v>-6.1999999999999886</v>
+      </c>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="3"/>
       <c r="T17" s="1"/>
-      <c r="U17" s="2"/>
-      <c r="V17" s="2"/>
-    </row>
-    <row r="18" spans="1:22">
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+    </row>
+    <row r="18" spans="1:24">
       <c r="A18">
         <v>900</v>
       </c>
@@ -85860,52 +86062,54 @@
       <c r="D18" s="1">
         <v>285.2</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="4">
         <v>282.8</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="4">
         <v>282.60000000000002</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="3">
+        <v>282</v>
+      </c>
+      <c r="H18" s="3">
+        <v>282</v>
+      </c>
+      <c r="I18" s="1">
         <f t="shared" si="0"/>
-        <v>1.144492131616591</v>
-      </c>
-      <c r="H18" s="1">
+        <v>0.85836909871243816</v>
+      </c>
+      <c r="J18" s="1">
         <f t="shared" si="1"/>
-        <v>1.0729613733905579</v>
-      </c>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18">
-        <v>900</v>
-      </c>
-      <c r="L18">
-        <v>944</v>
+        <v>0.85836909871243816</v>
+      </c>
+      <c r="K18" s="1"/>
+      <c r="L18" s="2">
+        <f t="shared" si="2"/>
+        <v>-2.3999999999999773</v>
       </c>
       <c r="M18" s="1">
-        <v>282.8</v>
-      </c>
-      <c r="N18" s="3">
-        <v>282.60000000000002</v>
-      </c>
-      <c r="O18" s="1">
-        <v>282.68799999999999</v>
-      </c>
-      <c r="P18" s="1">
-        <v>282.74200000000002</v>
-      </c>
-      <c r="Q18" s="3">
-        <v>282</v>
-      </c>
-      <c r="R18" s="3">
-        <v>282</v>
-      </c>
-      <c r="S18" s="1"/>
-      <c r="T18" s="1"/>
-      <c r="U18" s="2"/>
-      <c r="V18" s="2"/>
-    </row>
-    <row r="19" spans="1:22">
+        <f t="shared" si="3"/>
+        <v>-2.5999999999999659</v>
+      </c>
+      <c r="N18" s="1">
+        <f t="shared" si="4"/>
+        <v>-3.1999999999999886</v>
+      </c>
+      <c r="O18" s="4">
+        <f t="shared" si="5"/>
+        <v>-3.1999999999999886</v>
+      </c>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="3"/>
+      <c r="T18" s="3"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+    </row>
+    <row r="19" spans="1:24">
       <c r="A19">
         <v>900</v>
       </c>
@@ -85918,52 +86122,54 @@
       <c r="D19" s="1">
         <v>268.8</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="4">
         <v>264.8</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="4">
         <v>264.39999999999998</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19" s="3">
+        <v>263.39999999999998</v>
+      </c>
+      <c r="H19" s="3">
+        <v>263.39999999999998</v>
+      </c>
+      <c r="I19" s="1">
         <f t="shared" si="0"/>
-        <v>2.1604938271605025</v>
-      </c>
-      <c r="H19" s="1">
+        <v>1.620370370370366</v>
+      </c>
+      <c r="J19" s="1">
         <f t="shared" si="1"/>
-        <v>2.0061728395061684</v>
-      </c>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19">
-        <v>900</v>
-      </c>
-      <c r="L19">
-        <v>989</v>
+        <v>1.620370370370366</v>
+      </c>
+      <c r="K19" s="1"/>
+      <c r="L19" s="2">
+        <f t="shared" si="2"/>
+        <v>-4</v>
       </c>
       <c r="M19" s="1">
-        <v>264.8</v>
-      </c>
-      <c r="N19" s="3">
-        <v>264.39999999999998</v>
-      </c>
-      <c r="O19" s="1">
-        <v>265.01599999999996</v>
-      </c>
-      <c r="P19" s="1">
-        <v>264.93</v>
-      </c>
-      <c r="Q19" s="3">
-        <v>263.39999999999998</v>
-      </c>
-      <c r="R19" s="3">
-        <v>263.39999999999998</v>
-      </c>
-      <c r="S19" s="1"/>
-      <c r="T19" s="1"/>
-      <c r="U19" s="2"/>
-      <c r="V19" s="2"/>
-    </row>
-    <row r="20" spans="1:22">
+        <f t="shared" si="3"/>
+        <v>-4.4000000000000341</v>
+      </c>
+      <c r="N19" s="1">
+        <f t="shared" si="4"/>
+        <v>-5.4000000000000341</v>
+      </c>
+      <c r="O19" s="4">
+        <f t="shared" si="5"/>
+        <v>-5.4000000000000341</v>
+      </c>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="3"/>
+      <c r="T19" s="3"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+    </row>
+    <row r="20" spans="1:24">
       <c r="A20">
         <v>900</v>
       </c>
@@ -85976,52 +86182,54 @@
       <c r="D20" s="1">
         <v>250.6</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="4">
         <v>247</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="4">
         <v>247.4</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20" s="4">
+        <v>245</v>
+      </c>
+      <c r="H20" s="3">
+        <v>244.6</v>
+      </c>
+      <c r="I20" s="1">
         <f t="shared" si="0"/>
-        <v>2.6600166251039092</v>
-      </c>
-      <c r="H20" s="1">
+        <v>1.8287614297589385</v>
+      </c>
+      <c r="J20" s="1">
         <f t="shared" si="1"/>
-        <v>2.8262676641729061</v>
-      </c>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20">
-        <v>900</v>
-      </c>
-      <c r="L20">
-        <v>1034</v>
-      </c>
-      <c r="M20" s="3">
-        <v>247</v>
+        <v>1.6625103906899419</v>
+      </c>
+      <c r="K20" s="1"/>
+      <c r="L20" s="2">
+        <f t="shared" si="2"/>
+        <v>-3.5999999999999943</v>
+      </c>
+      <c r="M20" s="1">
+        <f t="shared" si="3"/>
+        <v>-3.1999999999999886</v>
       </c>
       <c r="N20" s="1">
-        <v>247.4</v>
-      </c>
-      <c r="O20" s="1">
-        <v>246.99799999999999</v>
-      </c>
-      <c r="P20" s="1">
-        <v>246.97999999999996</v>
-      </c>
-      <c r="Q20" s="1">
-        <v>245</v>
-      </c>
-      <c r="R20" s="3">
-        <v>244.6</v>
-      </c>
+        <f t="shared" si="4"/>
+        <v>-5.5999999999999943</v>
+      </c>
+      <c r="O20" s="4">
+        <f t="shared" si="5"/>
+        <v>-6</v>
+      </c>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
       <c r="S20" s="1"/>
-      <c r="T20" s="1"/>
-      <c r="U20" s="2"/>
-      <c r="V20" s="2"/>
-    </row>
-    <row r="21" spans="1:22">
+      <c r="T20" s="3"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2"/>
+    </row>
+    <row r="21" spans="1:24">
       <c r="A21">
         <v>900</v>
       </c>
@@ -86034,52 +86242,54 @@
       <c r="D21" s="1">
         <v>235.8</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="4">
         <v>232.4</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="4">
         <v>231</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21" s="4">
+        <v>229.6</v>
+      </c>
+      <c r="H21" s="3">
+        <v>229.4</v>
+      </c>
+      <c r="I21" s="1">
         <f t="shared" si="0"/>
-        <v>4.1218637992831617</v>
-      </c>
-      <c r="H21" s="1">
+        <v>2.8673835125448055</v>
+      </c>
+      <c r="J21" s="1">
         <f t="shared" si="1"/>
-        <v>3.4946236559139838</v>
-      </c>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21">
-        <v>900</v>
-      </c>
-      <c r="L21">
-        <v>1079</v>
+        <v>2.7777777777777857</v>
+      </c>
+      <c r="K21" s="1"/>
+      <c r="L21" s="2">
+        <f t="shared" si="2"/>
+        <v>-3.4000000000000057</v>
       </c>
       <c r="M21" s="1">
-        <v>232.4</v>
-      </c>
-      <c r="N21" s="3">
-        <v>231</v>
-      </c>
-      <c r="O21" s="1">
-        <v>231.96999999999997</v>
-      </c>
-      <c r="P21" s="1">
-        <v>231.958</v>
-      </c>
-      <c r="Q21" s="1">
-        <v>229.6</v>
-      </c>
-      <c r="R21" s="3">
-        <v>229.4</v>
-      </c>
+        <f t="shared" si="3"/>
+        <v>-4.8000000000000114</v>
+      </c>
+      <c r="N21" s="1">
+        <f t="shared" si="4"/>
+        <v>-6.2000000000000171</v>
+      </c>
+      <c r="O21" s="4">
+        <f t="shared" si="5"/>
+        <v>-6.4000000000000057</v>
+      </c>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
       <c r="S21" s="1"/>
-      <c r="T21" s="1"/>
-      <c r="U21" s="2"/>
-      <c r="V21" s="2"/>
-    </row>
-    <row r="22" spans="1:22">
+      <c r="T21" s="3"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="2"/>
+      <c r="X21" s="2"/>
+    </row>
+    <row r="22" spans="1:24">
       <c r="A22">
         <v>900</v>
       </c>
@@ -86092,52 +86302,54 @@
       <c r="D22" s="1">
         <v>219</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="4">
         <v>214.8</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="4">
         <v>214.2</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22" s="3">
+        <v>213</v>
+      </c>
+      <c r="H22" s="4">
+        <v>213.2</v>
+      </c>
+      <c r="I22" s="1">
         <f t="shared" si="0"/>
-        <v>4.27184466019418</v>
-      </c>
-      <c r="H22" s="1">
+        <v>3.3980582524271843</v>
+      </c>
+      <c r="J22" s="1">
         <f t="shared" si="1"/>
-        <v>3.9805825242718389</v>
-      </c>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22">
-        <v>900</v>
-      </c>
-      <c r="L22">
-        <v>1124</v>
+        <v>3.4951456310679556</v>
+      </c>
+      <c r="K22" s="1"/>
+      <c r="L22" s="2">
+        <f t="shared" si="2"/>
+        <v>-4.1999999999999886</v>
       </c>
       <c r="M22" s="1">
-        <v>214.8</v>
-      </c>
-      <c r="N22" s="3">
-        <v>214.2</v>
-      </c>
-      <c r="O22" s="1">
-        <v>215.31599999999997</v>
-      </c>
-      <c r="P22" s="1">
-        <v>215.86399999999998</v>
-      </c>
-      <c r="Q22" s="3">
-        <v>213</v>
-      </c>
-      <c r="R22" s="1">
-        <v>213.2</v>
-      </c>
-      <c r="S22" s="1"/>
+        <f t="shared" si="3"/>
+        <v>-4.8000000000000114</v>
+      </c>
+      <c r="N22" s="1">
+        <f t="shared" si="4"/>
+        <v>-6</v>
+      </c>
+      <c r="O22" s="4">
+        <f t="shared" si="5"/>
+        <v>-5.8000000000000114</v>
+      </c>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="3"/>
       <c r="T22" s="1"/>
-      <c r="U22" s="2"/>
-      <c r="V22" s="2"/>
-    </row>
-    <row r="23" spans="1:22">
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="2"/>
+      <c r="X22" s="2"/>
+    </row>
+    <row r="23" spans="1:24">
       <c r="A23">
         <v>1000</v>
       </c>
@@ -86150,52 +86362,54 @@
       <c r="D23" s="1">
         <v>317.39999999999998</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" s="4">
         <v>315.39999999999998</v>
       </c>
       <c r="F23" s="3">
         <v>314.60000000000002</v>
       </c>
-      <c r="G23" s="1">
+      <c r="G23" s="3">
+        <v>314.60000000000002</v>
+      </c>
+      <c r="H23" s="3">
+        <v>314.60000000000002</v>
+      </c>
+      <c r="I23" s="1">
         <f t="shared" si="0"/>
-        <v>1.0897435897435823</v>
-      </c>
-      <c r="H23" s="1">
+        <v>0.83333333333334059</v>
+      </c>
+      <c r="J23" s="1">
         <f t="shared" si="1"/>
         <v>0.83333333333334059</v>
       </c>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23">
-        <v>1000</v>
-      </c>
-      <c r="L23">
-        <v>1047</v>
+      <c r="K23" s="3"/>
+      <c r="L23" s="2">
+        <f t="shared" si="2"/>
+        <v>-2</v>
       </c>
       <c r="M23" s="1">
-        <v>315.39999999999998</v>
-      </c>
-      <c r="N23" s="3">
-        <v>314.60000000000002</v>
-      </c>
-      <c r="O23" s="1">
-        <v>315.91999999999996</v>
-      </c>
-      <c r="P23" s="1">
-        <v>315.76400000000001</v>
-      </c>
-      <c r="Q23" s="3">
-        <v>314.60000000000002</v>
-      </c>
-      <c r="R23" s="3">
-        <v>314.60000000000002</v>
-      </c>
-      <c r="S23" s="1"/>
-      <c r="T23" s="1"/>
-      <c r="U23" s="2"/>
-      <c r="V23" s="2"/>
-    </row>
-    <row r="24" spans="1:22">
+        <f t="shared" si="3"/>
+        <v>-2.7999999999999545</v>
+      </c>
+      <c r="N23" s="1">
+        <f t="shared" si="4"/>
+        <v>-2.7999999999999545</v>
+      </c>
+      <c r="O23" s="4">
+        <f t="shared" si="5"/>
+        <v>-2.7999999999999545</v>
+      </c>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2"/>
+    </row>
+    <row r="24" spans="1:24">
       <c r="A24">
         <v>1000</v>
       </c>
@@ -86208,52 +86422,54 @@
       <c r="D24" s="1">
         <v>299.60000000000002</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="4">
         <v>295.60000000000002</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F24" s="4">
         <v>296</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G24" s="4">
+        <v>294.39999999999998</v>
+      </c>
+      <c r="H24" s="3">
+        <v>294.2</v>
+      </c>
+      <c r="I24" s="1">
         <f t="shared" si="0"/>
-        <v>1.9310344827586285</v>
-      </c>
-      <c r="H24" s="1">
+        <v>1.517241379310337</v>
+      </c>
+      <c r="J24" s="1">
         <f t="shared" si="1"/>
-        <v>2.0689655172413794</v>
-      </c>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24">
-        <v>1000</v>
-      </c>
-      <c r="L24">
-        <v>1095</v>
-      </c>
-      <c r="M24" s="3">
-        <v>295.60000000000002</v>
+        <v>1.4482758620689615</v>
+      </c>
+      <c r="K24" s="1"/>
+      <c r="L24" s="2">
+        <f t="shared" si="2"/>
+        <v>-4</v>
+      </c>
+      <c r="M24" s="1">
+        <f t="shared" si="3"/>
+        <v>-3.6000000000000227</v>
       </c>
       <c r="N24" s="1">
-        <v>296</v>
-      </c>
-      <c r="O24" s="1">
-        <v>295.858</v>
-      </c>
-      <c r="P24" s="1">
-        <v>295.71600000000001</v>
-      </c>
-      <c r="Q24" s="1">
-        <v>294.39999999999998</v>
-      </c>
-      <c r="R24" s="3">
-        <v>294.2</v>
-      </c>
+        <f t="shared" si="4"/>
+        <v>-5.2000000000000455</v>
+      </c>
+      <c r="O24" s="4">
+        <f t="shared" si="5"/>
+        <v>-5.4000000000000341</v>
+      </c>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
       <c r="S24" s="1"/>
-      <c r="T24" s="1"/>
-      <c r="U24" s="2"/>
-      <c r="V24" s="2"/>
-    </row>
-    <row r="25" spans="1:22">
+      <c r="T24" s="3"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="2"/>
+      <c r="X24" s="2"/>
+    </row>
+    <row r="25" spans="1:24">
       <c r="A25">
         <v>1000</v>
       </c>
@@ -86266,52 +86482,54 @@
       <c r="D25" s="1">
         <v>283</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="4">
         <v>277.8</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F25" s="4">
         <v>278.39999999999998</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25" s="4">
+        <v>276.2</v>
+      </c>
+      <c r="H25" s="3">
+        <v>276</v>
+      </c>
+      <c r="I25" s="1">
         <f t="shared" si="0"/>
-        <v>2.4336283185840792</v>
-      </c>
-      <c r="H25" s="1">
+        <v>1.8436578171091444</v>
+      </c>
+      <c r="J25" s="1">
         <f t="shared" si="1"/>
-        <v>2.6548672566371638</v>
-      </c>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25">
-        <v>1000</v>
-      </c>
-      <c r="L25">
-        <v>1143</v>
-      </c>
-      <c r="M25" s="3">
-        <v>277.8</v>
+        <v>1.7699115044247828</v>
+      </c>
+      <c r="K25" s="1"/>
+      <c r="L25" s="2">
+        <f t="shared" si="2"/>
+        <v>-5.1999999999999886</v>
+      </c>
+      <c r="M25" s="1">
+        <f t="shared" si="3"/>
+        <v>-4.6000000000000227</v>
       </c>
       <c r="N25" s="1">
-        <v>278.39999999999998</v>
-      </c>
-      <c r="O25" s="1">
-        <v>278.01</v>
-      </c>
-      <c r="P25" s="1">
-        <v>277.94200000000001</v>
-      </c>
-      <c r="Q25" s="1">
-        <v>276.2</v>
-      </c>
-      <c r="R25" s="3">
-        <v>276</v>
-      </c>
+        <f t="shared" si="4"/>
+        <v>-6.8000000000000114</v>
+      </c>
+      <c r="O25" s="4">
+        <f t="shared" si="5"/>
+        <v>-7</v>
+      </c>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
       <c r="S25" s="1"/>
-      <c r="T25" s="1"/>
-      <c r="U25" s="2"/>
-      <c r="V25" s="2"/>
-    </row>
-    <row r="26" spans="1:22">
+      <c r="T25" s="3"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="2"/>
+      <c r="X25" s="2"/>
+    </row>
+    <row r="26" spans="1:24">
       <c r="A26">
         <v>1000</v>
       </c>
@@ -86324,52 +86542,54 @@
       <c r="D26" s="1">
         <v>264</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="4">
         <v>259.39999999999998</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26" s="4">
         <v>259.39999999999998</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G26" s="3">
+        <v>257.2</v>
+      </c>
+      <c r="H26" s="3">
+        <v>257.2</v>
+      </c>
+      <c r="I26" s="1">
         <f t="shared" si="0"/>
-        <v>3.3466135458167243</v>
-      </c>
-      <c r="H26" s="1">
+        <v>2.4701195219123462</v>
+      </c>
+      <c r="J26" s="1">
         <f t="shared" si="1"/>
-        <v>3.3466135458167243</v>
-      </c>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26">
-        <v>1000</v>
-      </c>
-      <c r="L26">
-        <v>1191</v>
-      </c>
-      <c r="M26" s="3">
-        <v>259.39999999999998</v>
-      </c>
-      <c r="N26" s="3">
-        <v>259.39999999999998</v>
-      </c>
-      <c r="O26" s="1">
-        <v>260.03999999999996</v>
-      </c>
-      <c r="P26" s="1">
-        <v>259.89</v>
-      </c>
-      <c r="Q26" s="3">
-        <v>257.2</v>
-      </c>
-      <c r="R26" s="3">
-        <v>257.2</v>
-      </c>
-      <c r="S26" s="1"/>
-      <c r="T26" s="1"/>
-      <c r="U26" s="2"/>
-      <c r="V26" s="2"/>
-    </row>
-    <row r="27" spans="1:22">
+        <v>2.4701195219123462</v>
+      </c>
+      <c r="K26" s="1"/>
+      <c r="L26" s="2">
+        <f t="shared" si="2"/>
+        <v>-4.6000000000000227</v>
+      </c>
+      <c r="M26" s="1">
+        <f t="shared" si="3"/>
+        <v>-4.6000000000000227</v>
+      </c>
+      <c r="N26" s="1">
+        <f t="shared" si="4"/>
+        <v>-6.8000000000000114</v>
+      </c>
+      <c r="O26" s="4">
+        <f t="shared" si="5"/>
+        <v>-6.8000000000000114</v>
+      </c>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="3"/>
+      <c r="T26" s="3"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="2"/>
+      <c r="X26" s="2"/>
+    </row>
+    <row r="27" spans="1:24">
       <c r="A27">
         <v>1000</v>
       </c>
@@ -86382,50 +86602,115 @@
       <c r="D27" s="1">
         <v>249.6</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="4">
         <v>244</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F27" s="4">
         <v>244.4</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G27" s="3">
+        <v>242.2</v>
+      </c>
+      <c r="H27" s="3">
+        <v>242.2</v>
+      </c>
+      <c r="I27" s="1">
         <f t="shared" si="0"/>
-        <v>3.7414965986394608</v>
-      </c>
-      <c r="H27" s="1">
+        <v>2.9761904761904763</v>
+      </c>
+      <c r="J27" s="1">
         <f t="shared" si="1"/>
-        <v>3.9115646258503474</v>
-      </c>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27">
-        <v>1000</v>
-      </c>
-      <c r="L27">
-        <v>1239</v>
-      </c>
-      <c r="M27" s="3">
-        <v>244</v>
+        <v>2.9761904761904763</v>
+      </c>
+      <c r="K27" s="1"/>
+      <c r="L27" s="2">
+        <f t="shared" si="2"/>
+        <v>-5.5999999999999943</v>
+      </c>
+      <c r="M27" s="1">
+        <f t="shared" si="3"/>
+        <v>-5.1999999999999886</v>
       </c>
       <c r="N27" s="1">
-        <v>244.4</v>
-      </c>
-      <c r="O27" s="1">
-        <v>244.72200000000004</v>
-      </c>
-      <c r="P27" s="1">
-        <v>245.01599999999999</v>
-      </c>
-      <c r="Q27" s="3">
-        <v>242.2</v>
-      </c>
-      <c r="R27" s="3">
-        <v>242.2</v>
-      </c>
-      <c r="S27" s="1"/>
-      <c r="T27" s="1"/>
-      <c r="U27" s="2"/>
-      <c r="V27" s="2"/>
+        <f t="shared" si="4"/>
+        <v>-7.4000000000000057</v>
+      </c>
+      <c r="O27" s="4">
+        <f t="shared" si="5"/>
+        <v>-7.4000000000000057</v>
+      </c>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="3"/>
+      <c r="T27" s="3"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="2"/>
+      <c r="X27" s="2"/>
+    </row>
+    <row r="29" spans="1:24">
+      <c r="K29" t="s">
+        <v>564</v>
+      </c>
+      <c r="L29" s="2">
+        <f>COUNTIF(L3:L27,"&lt;0")</f>
+        <v>24</v>
+      </c>
+      <c r="M29" s="1">
+        <f>COUNTIF(M3:M27,"&lt;0")</f>
+        <v>25</v>
+      </c>
+      <c r="N29" s="1">
+        <f t="shared" ref="N29:O29" si="6">COUNTIF(N3:N27,"&lt;0")</f>
+        <v>25</v>
+      </c>
+      <c r="O29" s="1">
+        <f t="shared" si="6"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24">
+      <c r="K30" t="s">
+        <v>565</v>
+      </c>
+      <c r="L30" s="2">
+        <f>COUNTIF(L3:L27,"&gt;0")</f>
+        <v>1</v>
+      </c>
+      <c r="M30" s="1">
+        <f>COUNTIF(M3:M27,"&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="N30" s="1">
+        <f t="shared" ref="N30:O30" si="7">COUNTIF(N3:N27,"&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="O30" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24">
+      <c r="K31" t="s">
+        <v>566</v>
+      </c>
+      <c r="L31">
+        <f>COUNTIF(L3:L27,"=0")</f>
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <f>COUNTIF(M3:M27,"=0")</f>
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <f t="shared" ref="N31:O31" si="8">COUNTIF(N3:N27,"=0")</f>
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -86437,8 +86722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -86455,10 +86740,10 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="I1" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -86469,19 +86754,19 @@
         <v>546</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>545</v>
@@ -86490,19 +86775,19 @@
         <v>546</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="L2" s="5" t="s">
+        <v>552</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>554</v>
       </c>
-      <c r="M2" s="5" t="s">
-        <v>558</v>
-      </c>
       <c r="N2" s="5" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="3" spans="1:15">

</xml_diff>